<commit_message>
jo/udpate generate data and training
</commit_message>
<xml_diff>
--- a/config/optimization_engine/ml_models/process_a-example-input-model.xlsx
+++ b/config/optimization_engine/ml_models/process_a-example-input-model.xlsx
@@ -460,16 +460,16 @@
         <v>29</v>
       </c>
       <c r="B2" t="n">
-        <v>8.036720768991145</v>
+        <v>80.38067699035999</v>
       </c>
       <c r="C2" t="n">
-        <v>1.865700588860358</v>
+        <v>18.85621941051061</v>
       </c>
       <c r="D2" t="n">
-        <v>8.925589984899778</v>
+        <v>89.25706332453439</v>
       </c>
       <c r="E2" t="n">
-        <v>5.393422419156507</v>
+        <v>54.08160640019621</v>
       </c>
     </row>
   </sheetData>

</xml_diff>